<commit_message>
test with pre-commit post-commit
</commit_message>
<xml_diff>
--- a/excel-test.xlsx
+++ b/excel-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debra/UChicago/Excel/laughing-disco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A89112A-EF10-9C49-A8C7-81AB8DF436E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2E2A28-7EA8-B847-BA09-46140ADCA485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-50480" yWindow="-2380" windowWidth="35840" windowHeight="20760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1628,7 +1628,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1775,7 +1775,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C9" s="27">
         <v>8</v>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="E9" s="30">
         <f>SUM(B9,C9,D9)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="13"/>
@@ -1832,14 +1832,14 @@
         <v>3</v>
       </c>
       <c r="C12" s="25">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D12" s="25">
         <v>3</v>
       </c>
       <c r="E12" s="30">
         <f>SUM(B12,C12,D12)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="11"/>

</xml_diff>

<commit_message>
test with post-commit hook only
</commit_message>
<xml_diff>
--- a/excel-test.xlsx
+++ b/excel-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debra/UChicago/Excel/laughing-disco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB99914-C8B5-7045-8E19-886DEFAAB7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44860053-49CF-1F48-9691-3EEF1DDCC748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50480" yWindow="-2380" windowWidth="35840" windowHeight="20760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-58440" yWindow="-2040" windowWidth="16960" windowHeight="20760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -365,7 +365,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -427,15 +427,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1628,7 +1619,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1638,15 +1629,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -1659,7 +1650,7 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4"/>
@@ -1669,16 +1660,19 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="25">
         <v>1</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="26">
         <v>2</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="26">
         <v>3</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="27">
+        <f>SUM(B3,C3,D3)</f>
+        <v>6</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
@@ -1686,16 +1680,19 @@
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="21">
         <v>1</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="22">
         <v>2</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <v>3</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="27">
+        <f>SUM(B4,C4,D4)</f>
+        <v>6</v>
+      </c>
       <c r="F4" s="10"/>
       <c r="G4" s="11"/>
     </row>
@@ -1703,18 +1700,18 @@
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="26">
-        <v>1</v>
-      </c>
-      <c r="C5" s="27">
+      <c r="B5" s="23">
+        <v>11</v>
+      </c>
+      <c r="C5" s="24">
         <v>5</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="24">
         <v>3</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="27">
         <f>SUM(B5,C5,D5)</f>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="13"/>
@@ -1723,16 +1720,19 @@
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="21">
         <v>1</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="22">
         <v>2</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <v>3</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="27">
+        <f>SUM(B6,C6,D6)</f>
+        <v>6</v>
+      </c>
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
     </row>
@@ -1740,16 +1740,19 @@
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="23">
         <v>1</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="24">
         <v>2</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="24">
         <v>3</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="27">
+        <f>SUM(B7,C7,D7)</f>
+        <v>6</v>
+      </c>
       <c r="F7" s="12"/>
       <c r="G7" s="13"/>
     </row>
@@ -1757,16 +1760,19 @@
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="21">
         <v>1</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="22">
         <v>2</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="22">
         <v>3</v>
       </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="27">
+        <f>SUM(B8,C8,D8)</f>
+        <v>6</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
     </row>
@@ -1774,18 +1780,18 @@
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="26">
-        <v>4</v>
-      </c>
-      <c r="C9" s="27">
+      <c r="B9" s="23">
+        <v>9</v>
+      </c>
+      <c r="C9" s="24">
         <v>15</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="24">
         <v>3</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="27">
         <f>SUM(B9,C9,D9)</f>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="13"/>
@@ -1794,16 +1800,19 @@
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="21">
         <v>1</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="22">
         <v>2</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="22">
         <v>3</v>
       </c>
-      <c r="E10" s="22"/>
+      <c r="E10" s="27">
+        <f>SUM(B10,C10,D10)</f>
+        <v>6</v>
+      </c>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
     </row>
@@ -1811,16 +1820,19 @@
       <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="26">
-        <v>1</v>
-      </c>
-      <c r="C11" s="27">
+      <c r="B11" s="23">
+        <v>4</v>
+      </c>
+      <c r="C11" s="24">
         <v>2</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="24">
         <v>3</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="27">
+        <f>SUM(B11,C11,D11)</f>
+        <v>9</v>
+      </c>
       <c r="F11" s="12"/>
       <c r="G11" s="13"/>
     </row>
@@ -1828,16 +1840,16 @@
       <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="21">
         <v>3</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="22">
         <v>6</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="22">
         <v>3</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="27">
         <f>SUM(B12,C12,D12)</f>
         <v>12</v>
       </c>

</xml_diff>